<commit_message>
results diff and heatmaps
</commit_message>
<xml_diff>
--- a/results/weights/data_weight.xlsx
+++ b/results/weights/data_weight.xlsx
@@ -5,17 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_f_v_beerendonk_student_tue_nl/Documents/Desktop/final project/final_thesis/experiments/v3/weights/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/p_f_v_beerendonk_student_tue_nl/Documents/Desktop/final project/final_thesis/final_thesis_partitioning/results/weights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="424" documentId="11_F25DC773A252ABDACC104837699F7C7C5ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9E82559-83C4-4A0B-86B3-B989CD0CCB14}"/>
+  <xr:revisionPtr revIDLastSave="430" documentId="11_F25DC773A252ABDACC104837699F7C7C5ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{044A248F-21C0-40EA-BF71-75E8AAC1B4DA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tue_logo" sheetId="1" r:id="rId1"/>
     <sheet name="propeller" sheetId="3" r:id="rId2"/>
-    <sheet name="donut" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>util</t>
   </si>
@@ -61,22 +60,7 @@
     <t>runtime</t>
   </si>
   <si>
-    <t>WEEE WOO</t>
-  </si>
-  <si>
-    <t>Break at 12parts is on</t>
-  </si>
-  <si>
-    <t>so probably, this is just plain wrong</t>
-  </si>
-  <si>
-    <t>or model is too large for volume?</t>
-  </si>
-  <si>
     <t>MULTIPLE RUNS V V V</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -414,23 +398,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="2.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -440,20 +423,20 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,20 +446,20 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>6</v>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.97389715736501203</v>
       </c>
       <c r="F2" s="3">
-        <v>0.97389715736501203</v>
-      </c>
-      <c r="G2" s="3">
         <v>0.86224016877661402</v>
       </c>
-      <c r="H2" s="5">
+      <c r="G2" s="5">
         <v>3653.7578358650198</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -486,20 +469,20 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>6</v>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.97389715736501203</v>
       </c>
       <c r="F3" s="3">
-        <v>0.97389715736501203</v>
-      </c>
-      <c r="G3" s="3">
         <v>0.86224016877661402</v>
       </c>
-      <c r="H3" s="5">
+      <c r="G3" s="5">
         <v>3584.0071699619202</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -509,20 +492,20 @@
       <c r="C4">
         <v>1E-4</v>
       </c>
-      <c r="E4">
+      <c r="D4">
         <v>4</v>
       </c>
+      <c r="E4" s="3">
+        <v>0.97131508852188098</v>
+      </c>
       <c r="F4" s="3">
-        <v>0.97131508852188098</v>
-      </c>
-      <c r="G4" s="3">
         <v>0.27446622103629298</v>
       </c>
-      <c r="H4" s="5">
+      <c r="G4" s="5">
         <v>2516.0680644512099</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -532,20 +515,20 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>6</v>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.97389715736501203</v>
       </c>
       <c r="F5" s="3">
-        <v>0.97389715736501203</v>
-      </c>
-      <c r="G5" s="3">
         <v>0.86224016877661402</v>
       </c>
-      <c r="H5" s="5">
+      <c r="G5" s="5">
         <v>3575.6227102279599</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -555,20 +538,20 @@
       <c r="C6">
         <v>1E-4</v>
       </c>
-      <c r="E6">
-        <v>6</v>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.97416305109380397</v>
       </c>
       <c r="F6" s="3">
-        <v>0.97416305109380397</v>
-      </c>
-      <c r="G6" s="3">
         <v>0.30498869022916397</v>
       </c>
-      <c r="H6" s="5">
+      <c r="G6" s="5">
         <v>3675.7799034118598</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -578,20 +561,20 @@
       <c r="C7">
         <v>1E-3</v>
       </c>
-      <c r="E7">
+      <c r="D7">
         <v>4</v>
       </c>
+      <c r="E7" s="3">
+        <v>0.97131508852188098</v>
+      </c>
       <c r="F7" s="3">
-        <v>0.97131508852188098</v>
-      </c>
-      <c r="G7" s="3">
         <v>0.27446622103629298</v>
       </c>
-      <c r="H7" s="5">
+      <c r="G7" s="5">
         <v>2436.20756483078</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -601,20 +584,20 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="E8">
-        <v>6</v>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.97389715736501203</v>
       </c>
       <c r="F8" s="3">
-        <v>0.97389715736501203</v>
-      </c>
-      <c r="G8" s="3">
         <v>0.86224016877661402</v>
       </c>
-      <c r="H8" s="5">
+      <c r="G8" s="5">
         <v>3658.9366443157101</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -624,20 +607,20 @@
       <c r="C9">
         <v>1E-4</v>
       </c>
-      <c r="E9">
-        <v>6</v>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.97386962864108395</v>
       </c>
       <c r="F9" s="3">
-        <v>0.97386962864108395</v>
-      </c>
-      <c r="G9" s="3">
         <v>0.48070598087238903</v>
       </c>
-      <c r="H9" s="5">
+      <c r="G9" s="5">
         <v>3582.7072198390902</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -647,20 +630,20 @@
       <c r="C10">
         <v>1E-3</v>
       </c>
-      <c r="E10">
-        <v>6</v>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.97416305109380397</v>
       </c>
       <c r="F10" s="3">
-        <v>0.97416305109380397</v>
-      </c>
-      <c r="G10" s="3">
         <v>0.30498869022916397</v>
       </c>
-      <c r="H10" s="5">
+      <c r="G10" s="5">
         <v>3509.22427821159</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -670,20 +653,20 @@
       <c r="C11">
         <v>0.01</v>
       </c>
-      <c r="E11">
+      <c r="D11">
         <v>4</v>
       </c>
+      <c r="E11" s="3">
+        <v>0.97131508852188098</v>
+      </c>
       <c r="F11" s="3">
-        <v>0.97131508852188098</v>
-      </c>
-      <c r="G11" s="3">
         <v>0.27446622103629298</v>
       </c>
-      <c r="H11" s="5">
+      <c r="G11" s="5">
         <v>2519.6604101657799</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -693,20 +676,20 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="E12">
-        <v>6</v>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.97389715736501203</v>
       </c>
       <c r="F12" s="3">
-        <v>0.97389715736501203</v>
-      </c>
-      <c r="G12" s="3">
         <v>0.86224016877661402</v>
       </c>
-      <c r="H12" s="5">
+      <c r="G12" s="5">
         <v>3565.8243687152799</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -716,20 +699,20 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="E13">
-        <v>6</v>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.97389715736501203</v>
       </c>
       <c r="F13" s="3">
-        <v>0.97389715736501203</v>
-      </c>
-      <c r="G13" s="3">
         <v>0.86224016877661402</v>
       </c>
-      <c r="H13" s="5">
+      <c r="G13" s="5">
         <v>3563.81428289413</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -739,20 +722,20 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="E14">
-        <v>6</v>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.97389715736501203</v>
       </c>
       <c r="F14" s="3">
-        <v>0.97389715736501203</v>
-      </c>
-      <c r="G14" s="3">
         <v>0.86224016877661402</v>
       </c>
-      <c r="H14" s="5">
+      <c r="G14" s="5">
         <v>3554.2772974967902</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -762,20 +745,20 @@
       <c r="C15">
         <v>1E-4</v>
       </c>
-      <c r="E15">
-        <v>6</v>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.97402432787855397</v>
       </c>
       <c r="F15" s="3">
-        <v>0.97402432787855397</v>
-      </c>
-      <c r="G15" s="3">
         <v>0.40492312207683201</v>
       </c>
-      <c r="H15" s="5">
+      <c r="G15" s="5">
         <v>3531.5790393352499</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -785,20 +768,20 @@
       <c r="C16">
         <v>1E-4</v>
       </c>
-      <c r="E16">
+      <c r="D16">
         <v>4</v>
       </c>
+      <c r="E16" s="3">
+        <v>0.98039199409877298</v>
+      </c>
       <c r="F16" s="3">
-        <v>0.98039199409877298</v>
-      </c>
-      <c r="G16" s="3">
         <v>0.18419614537915799</v>
       </c>
-      <c r="H16" s="5">
+      <c r="G16" s="5">
         <v>2291.9974608421298</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -808,20 +791,20 @@
       <c r="C17">
         <v>1E-4</v>
       </c>
-      <c r="E17">
-        <v>6</v>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.97438266426097297</v>
       </c>
       <c r="F17" s="3">
-        <v>0.97438266426097297</v>
-      </c>
-      <c r="G17" s="3">
         <v>0.29842517204345897</v>
       </c>
-      <c r="H17" s="5">
+      <c r="G17" s="5">
         <v>3500.3609049320198</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -831,23 +814,20 @@
       <c r="C18">
         <v>1E-3</v>
       </c>
-      <c r="E18">
+      <c r="D18">
         <v>4</v>
       </c>
+      <c r="E18" s="3">
+        <v>0.98039199409877298</v>
+      </c>
       <c r="F18" s="3">
-        <v>0.98039199409877298</v>
-      </c>
-      <c r="G18" s="3">
         <v>0.18419614537915799</v>
       </c>
-      <c r="H18" s="5">
+      <c r="G18" s="5">
         <v>2333.3097577095</v>
       </c>
-      <c r="I18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -857,20 +837,20 @@
       <c r="C19">
         <v>1E-3</v>
       </c>
-      <c r="E19">
-        <v>6</v>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.97438266426097297</v>
       </c>
       <c r="F19" s="3">
-        <v>0.97438266426097297</v>
-      </c>
-      <c r="G19" s="3">
         <v>0.29842517204345897</v>
       </c>
-      <c r="H19" s="5">
+      <c r="G19" s="5">
         <v>3525.7109029293001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -880,50 +860,50 @@
       <c r="C20">
         <v>0.01</v>
       </c>
-      <c r="E20">
+      <c r="D20">
         <v>4</v>
       </c>
+      <c r="E20" s="3">
+        <v>0.98039199409877298</v>
+      </c>
       <c r="F20" s="3">
-        <v>0.98039199409877298</v>
-      </c>
-      <c r="G20" s="3">
         <v>0.18419614537915799</v>
       </c>
-      <c r="H20" s="5">
+      <c r="G20" s="5">
         <v>2334.98624467849</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1</v>
       </c>
@@ -937,7 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6B15C5-E4E2-4B88-B767-86BF3C3E75E2}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1626,7 +1606,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1654,424 +1634,6 @@
       <c r="I33" s="5">
         <f>H33/3600</f>
         <v>13.570230373409055</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC689D0-FE1A-4B8B-96D1-764CB5B844E2}">
-  <dimension ref="A1:I30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="2.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.99877380284464901</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1.04097204009109</v>
-      </c>
-      <c r="H2" s="5">
-        <v>18654.744856834401</v>
-      </c>
-      <c r="I2" s="5">
-        <f>H2/3600</f>
-        <v>5.181873571342889</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1E-4</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <f t="shared" ref="I3:I17" si="0">H3/3600</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1E-4</v>
-      </c>
-      <c r="C4">
-        <v>1E-4</v>
-      </c>
-      <c r="E4" s="5">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.99997533398921801</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.340452459229386</v>
-      </c>
-      <c r="H4" s="5">
-        <v>20887.7067661285</v>
-      </c>
-      <c r="I4" s="5">
-        <f t="shared" si="0"/>
-        <v>5.8021407683690276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1E-3</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1E-3</v>
-      </c>
-      <c r="C6">
-        <v>1E-4</v>
-      </c>
-      <c r="E6" s="5">
-        <v>12</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.99997533398921801</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.340452459229386</v>
-      </c>
-      <c r="H6" s="5">
-        <v>21287.363414287502</v>
-      </c>
-      <c r="I6" s="5">
-        <f t="shared" si="0"/>
-        <v>5.9131565039687501</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>0.01</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>0.01</v>
-      </c>
-      <c r="C8">
-        <v>1E-4</v>
-      </c>
-      <c r="E8" s="5">
-        <v>12</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.99432221210762095</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1.0681777066656699</v>
-      </c>
-      <c r="H8" s="5">
-        <v>18312.623818874301</v>
-      </c>
-      <c r="I8" s="5">
-        <f t="shared" si="0"/>
-        <v>5.086839949687306</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>0.01</v>
-      </c>
-      <c r="C9">
-        <v>1E-3</v>
-      </c>
-      <c r="E9" s="5">
-        <v>12</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.99999999682621199</v>
-      </c>
-      <c r="G9" s="3">
-        <v>8.7163254472062399E-2</v>
-      </c>
-      <c r="H9" s="5">
-        <v>148263.06007480601</v>
-      </c>
-      <c r="I9" s="5">
-        <f t="shared" si="0"/>
-        <v>41.184183354112783</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>0.1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="I10" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>0.1</v>
-      </c>
-      <c r="C11">
-        <v>1E-4</v>
-      </c>
-      <c r="E11" s="5">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.99426285088869204</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1.05852001066843</v>
-      </c>
-      <c r="H11" s="5">
-        <v>16908.686120748502</v>
-      </c>
-      <c r="I11" s="5">
-        <f t="shared" si="0"/>
-        <v>4.6968572557634731</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>0.1</v>
-      </c>
-      <c r="C12">
-        <v>1E-3</v>
-      </c>
-      <c r="E12" s="5">
-        <v>12</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.99432221210762095</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1.0681777066656699</v>
-      </c>
-      <c r="H12" s="5">
-        <v>17864.402934551199</v>
-      </c>
-      <c r="I12" s="5">
-        <f t="shared" si="0"/>
-        <v>4.9623341484864438</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>0.1</v>
-      </c>
-      <c r="C13">
-        <v>0.01</v>
-      </c>
-      <c r="E13" s="5">
-        <v>12</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.99997533398921801</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.340452459229386</v>
-      </c>
-      <c r="H13" s="5">
-        <v>21121.621448516798</v>
-      </c>
-      <c r="I13" s="5">
-        <f t="shared" si="0"/>
-        <v>5.8671170690324441</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>0.05</v>
-      </c>
-      <c r="C14">
-        <v>1E-4</v>
-      </c>
-      <c r="E14" s="5">
-        <v>12</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.99426285088869204</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1.05852001066843</v>
-      </c>
-      <c r="H14" s="5">
-        <v>16805.917622327801</v>
-      </c>
-      <c r="I14" s="5">
-        <f t="shared" si="0"/>
-        <v>4.6683104506466115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="I17" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G27" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G28" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G29" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="G30" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>